<commit_message>
lat to long and vice versa
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -9,7 +9,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mjrZxk4qlSsK+1+Fef1AAyp2UrURQ=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mhAOjc6Fc8WHXt/nuor8LQ/vVVzPA=="/>
     </ext>
   </extLst>
 </workbook>
@@ -39,13 +39,13 @@
     <t>Phone Number</t>
   </si>
   <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Longtitude</t>
+    <t>ProfilePicURL</t>
   </si>
   <si>
     <t>Latitude</t>
+  </si>
+  <si>
+    <t>Longitude</t>
   </si>
   <si>
     <t>Map URL</t>
@@ -105,15 +105,18 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="top"/>
+    </xf>
     <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center" readingOrder="0" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -358,13 +361,13 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">

</xml_diff>